<commit_message>
Add Source Links Sheet.
</commit_message>
<xml_diff>
--- a/DataEngineProgress.xlsx
+++ b/DataEngineProgress.xlsx
@@ -4,19 +4,20 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Data Boosting Notes" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet1" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjhOUFrU7nBpwf7fLQUotT9Zv8MPQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhoNuh6ed6ej+EarF0ZDu4DCoFIIw=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Engine Iteration Num:</t>
   </si>
@@ -63,14 +64,39 @@
     <t>R' - Recyclables</t>
   </si>
   <si>
-    <t>Dumped everything into trash - couldn't generalize</t>
+    <t>Dumped everything into trash - couldn't generalize. This iteration added 25,000 images. Will reevaluate the weighting issue after retraining in next iteration.</t>
+  </si>
+  <si>
+    <t>Source Links:</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/moezabid/bottles-and-cans</t>
+  </si>
+  <si>
+    <t>https://medium.com/@ringlayer/cardboard-box-detection-using-retinanet-keras-5d4f331d9d15</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/asdasdasasdas/garbage-classification</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">DuckDuck Go Scraper - </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://colab.research.google.com/github/joedockrill/image-scraper/blob/master/ImageScraper.ipynb</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -90,6 +116,10 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -125,6 +155,12 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" textRotation="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -134,6 +170,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -393,7 +433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" ht="48.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -409,7 +449,7 @@
       <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1420,4 +1460,59 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="24.11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
+  </hyperlinks>
+  <drawing r:id="rId6"/>
+</worksheet>
 </file>
</xml_diff>